<commit_message>
fix: cannot import data from 'Z' and subsequent columns
Refs: #129
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\repos\sbb\ch.sbb.polarion.extension.excel-importer\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sbb\rep\_github\ch.sbb.polarion.extension.excel-importer\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25BD95E-F6DC-45A7-8B28-0507E60D4612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F385C8-0736-46C1-9213-D7F958611457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="2085" windowWidth="21975" windowHeight="11850" activeTab="1" xr2:uid="{27913358-3868-4E49-A128-87CEC9A6139D}"/>
+    <workbookView xWindow="2895" yWindow="2790" windowWidth="24870" windowHeight="11580" activeTab="2" xr2:uid="{27913358-3868-4E49-A128-87CEC9A6139D}"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" r:id="rId1"/>
     <sheet name="empty" sheetId="2" r:id="rId2"/>
+    <sheet name="wide" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>a1</t>
   </si>
@@ -59,6 +60,30 @@
   </si>
   <si>
     <t>d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
+  </si>
+  <si>
+    <t>aaa1</t>
+  </si>
+  <si>
+    <t>aa1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>bb2</t>
+  </si>
+  <si>
+    <t>bbb2</t>
   </si>
 </sst>
 </file>
@@ -455,12 +480,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC43F9B3-CF0E-44D0-85A6-19FEFF4C254A}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311BA04E-1EAA-4D91-8C5A-DE64F92E04F0}">
+  <dimension ref="A1:BBB2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="BAE1" workbookViewId="0">
+      <selection activeCell="BAZ3" sqref="BAZ3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:703 1406:1406" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AAA1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:703 1406:1406" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BBB2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: cannot import data from 'Z' and subsequent columns (#130)
Refs: #129
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\repos\sbb\ch.sbb.polarion.extension.excel-importer\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sbb\rep\_github\ch.sbb.polarion.extension.excel-importer\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25BD95E-F6DC-45A7-8B28-0507E60D4612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F385C8-0736-46C1-9213-D7F958611457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="2085" windowWidth="21975" windowHeight="11850" activeTab="1" xr2:uid="{27913358-3868-4E49-A128-87CEC9A6139D}"/>
+    <workbookView xWindow="2895" yWindow="2790" windowWidth="24870" windowHeight="11580" activeTab="2" xr2:uid="{27913358-3868-4E49-A128-87CEC9A6139D}"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" r:id="rId1"/>
     <sheet name="empty" sheetId="2" r:id="rId2"/>
+    <sheet name="wide" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>a1</t>
   </si>
@@ -59,6 +60,30 @@
   </si>
   <si>
     <t>d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
+  </si>
+  <si>
+    <t>aaa1</t>
+  </si>
+  <si>
+    <t>aa1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>bb2</t>
+  </si>
+  <si>
+    <t>bbb2</t>
   </si>
 </sst>
 </file>
@@ -455,12 +480,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC43F9B3-CF0E-44D0-85A6-19FEFF4C254A}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311BA04E-1EAA-4D91-8C5A-DE64F92E04F0}">
+  <dimension ref="A1:BBB2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="BAE1" workbookViewId="0">
+      <selection activeCell="BAZ3" sqref="BAZ3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:703 1406:1406" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AAA1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:703 1406:1406" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BBB2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: import test steps
Refs: #169
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sbb\rep\_github\ch.sbb.polarion.extension.excel-importer\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F385C8-0736-46C1-9213-D7F958611457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C996C68-893A-4A1F-B847-431CADEFB705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2790" windowWidth="24870" windowHeight="11580" activeTab="2" xr2:uid="{27913358-3868-4E49-A128-87CEC9A6139D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{27913358-3868-4E49-A128-87CEC9A6139D}"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" r:id="rId1"/>
     <sheet name="empty" sheetId="2" r:id="rId2"/>
     <sheet name="wide" sheetId="3" r:id="rId3"/>
+    <sheet name="merged_ok" sheetId="5" r:id="rId4"/>
+    <sheet name="merged_fail" sheetId="4" r:id="rId5"/>
+    <sheet name="merged_mixed" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,12 +34,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>a1</t>
   </si>
@@ -84,6 +90,105 @@
   </si>
   <si>
     <t>bbb2</t>
+  </si>
+  <si>
+    <t>Header 1</t>
+  </si>
+  <si>
+    <t>Header 2</t>
+  </si>
+  <si>
+    <t>Header 3</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>These</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>will</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>skipped</t>
+  </si>
+  <si>
+    <t>C merged</t>
+  </si>
+  <si>
+    <t>B merged</t>
+  </si>
+  <si>
+    <t>A1-3</t>
+  </si>
+  <si>
+    <t>C1-3+D1-3</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>A5-6</t>
+  </si>
+  <si>
+    <t>B5-6</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>b6</t>
+  </si>
+  <si>
+    <t>b7</t>
+  </si>
+  <si>
+    <t>c6</t>
+  </si>
+  <si>
+    <t>c7</t>
+  </si>
+  <si>
+    <t>a8-9</t>
+  </si>
+  <si>
+    <t>b8-9</t>
+  </si>
+  <si>
+    <t>c8-9</t>
   </si>
 </sst>
 </file>
@@ -119,8 +224,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647ABFDD-59B6-4BED-B50F-F2147479FF3B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -515,7 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311BA04E-1EAA-4D91-8C5A-DE64F92E04F0}">
   <dimension ref="A1:BBB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BAE1" workbookViewId="0">
+    <sheetView topLeftCell="BAE1" workbookViewId="0">
       <selection activeCell="BAZ3" sqref="BAZ3"/>
     </sheetView>
   </sheetViews>
@@ -546,4 +654,250 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEB439C-3305-43F6-AFB4-9095660BA625}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D09DE0-3847-44B9-836C-D50716CF0C0D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DEB2FF0-D8BE-4BFE-921E-BEF18A4D2956}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:D3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: import test steps (#170)
Refs: #169
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sbb\rep\_github\ch.sbb.polarion.extension.excel-importer\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F385C8-0736-46C1-9213-D7F958611457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C996C68-893A-4A1F-B847-431CADEFB705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2790" windowWidth="24870" windowHeight="11580" activeTab="2" xr2:uid="{27913358-3868-4E49-A128-87CEC9A6139D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{27913358-3868-4E49-A128-87CEC9A6139D}"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" r:id="rId1"/>
     <sheet name="empty" sheetId="2" r:id="rId2"/>
     <sheet name="wide" sheetId="3" r:id="rId3"/>
+    <sheet name="merged_ok" sheetId="5" r:id="rId4"/>
+    <sheet name="merged_fail" sheetId="4" r:id="rId5"/>
+    <sheet name="merged_mixed" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,12 +34,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>a1</t>
   </si>
@@ -84,6 +90,105 @@
   </si>
   <si>
     <t>bbb2</t>
+  </si>
+  <si>
+    <t>Header 1</t>
+  </si>
+  <si>
+    <t>Header 2</t>
+  </si>
+  <si>
+    <t>Header 3</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>These</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>will</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>skipped</t>
+  </si>
+  <si>
+    <t>C merged</t>
+  </si>
+  <si>
+    <t>B merged</t>
+  </si>
+  <si>
+    <t>A1-3</t>
+  </si>
+  <si>
+    <t>C1-3+D1-3</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>A5-6</t>
+  </si>
+  <si>
+    <t>B5-6</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>b6</t>
+  </si>
+  <si>
+    <t>b7</t>
+  </si>
+  <si>
+    <t>c6</t>
+  </si>
+  <si>
+    <t>c7</t>
+  </si>
+  <si>
+    <t>a8-9</t>
+  </si>
+  <si>
+    <t>b8-9</t>
+  </si>
+  <si>
+    <t>c8-9</t>
   </si>
 </sst>
 </file>
@@ -119,8 +224,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647ABFDD-59B6-4BED-B50F-F2147479FF3B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -515,7 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311BA04E-1EAA-4D91-8C5A-DE64F92E04F0}">
   <dimension ref="A1:BBB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BAE1" workbookViewId="0">
+    <sheetView topLeftCell="BAE1" workbookViewId="0">
       <selection activeCell="BAZ3" sqref="BAZ3"/>
     </sheetView>
   </sheetViews>
@@ -546,4 +654,250 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEB439C-3305-43F6-AFB4-9095660BA625}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D09DE0-3847-44B9-836C-D50716CF0C0D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DEB2FF0-D8BE-4BFE-921E-BEF18A4D2956}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:D3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>